<commit_message>
Started work on globe visualization with brush things, i don't like writing these comments
</commit_message>
<xml_diff>
--- a/data/OECD_betterLifeIndex.xlsx
+++ b/data/OECD_betterLifeIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\pythonProject\CSC3833_Coursework_1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D30921-B64E-4088-B138-960D765D49FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E009703D-6FFD-4E09-8C9A-35EB539053ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="2625" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4275" yWindow="2595" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OECD.Stat export" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="128">
   <si>
     <t>&lt;?xml version="1.0" encoding="utf-16"?&gt;&lt;WebTableParameter xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns="http://stats.oecd.org/OECDStatWS/2004/03/01/"&gt;&lt;DataTable Code="BLI" HasMetadata="true"&gt;&lt;Name LocaleIsoCode="en"&gt;Better Life Index&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Indicateur du vivre mieux&lt;/Name&gt;&lt;Dimension Code="LOCATION" HasMetadata="false" CommonCode="LOCATION" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Country&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Pays&lt;/Name&gt;&lt;Member Code="AUS" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Australia&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Australie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="AUT" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Austria&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Autriche&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="BEL" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Belgium&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Belgique&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="CAN" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Canada&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Canada&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="CHL" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Chile&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Chili&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="COL" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Colombia&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Colombie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="CRI" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Costa Rica&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Costa Rica&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="CZE" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Czech Republic&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;République tchèque&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="DNK" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Denmark&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Danemark&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="EST" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Estonia&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Estonie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="FIN" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Finland&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Finlande&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="FRA" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;France&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;France&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="DEU" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Germany&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Allemagne&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="GRC" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Greece&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Grèce&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="HUN" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Hungary&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Hongrie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="ISL" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Iceland&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Islande&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="IRL" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Ireland&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Irlande&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="ISR" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Israel&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Israël&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="ITA" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Italy&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Italie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="JPN" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Japan&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Japon&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="KOR" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Korea&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Corée&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="LVA" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Latvia&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Lettonie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="LTU" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Lithuania&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Lituanie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="LUX" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Luxembourg&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Luxembourg&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="MEX" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Mexico&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Mexique&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="NLD" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Netherlands&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Pays-Bas&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="NZL" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;New Zealand&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Nouvelle-Zélande&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="NOR" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Norway&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Norvège&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="POL" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Poland&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Pologne&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="PRT" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Portugal&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Portugal&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="SVK" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Slovak Republic&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;République slovaque&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="SVN" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Slovenia&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Slovénie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="ESP" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Spain&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Espagne&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="SWE" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Sweden&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Suède&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="CHE" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Switzerland&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Suisse&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="TUR" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Türkiye&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Türkiye&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="GBR" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;United Kingdom&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Royaume-Uni&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="USA" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;United States&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;États-Unis&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="OECD" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;OECD - Total&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;OCDE - Total&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="NMEC" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Non-OECD Economies&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Économies non-OCDE&lt;/Name&gt;&lt;ChildMember Code="BRA" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Brazil&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Brésil&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="RUS" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Russia&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Russie&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="ZAF" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;South Africa&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Afrique du Sud&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="INDICATOR" HasMetadata="false" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Indicator&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Indicateur&lt;/Name&gt;&lt;Member Code="HO" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Housing&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Logement&lt;/Name&gt;&lt;ChildMember Code="HO_BASE" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0" IsDisplayed="true"&gt;&lt;Name LocaleIsoCode="en"&gt;Dwellings without basic facilities&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Logements sans équipements sanitaires de base&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="HO_HISH" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Housing expenditure&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Coût du logement&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="HO_NUMR" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Rooms per person&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Nombre de pièces par personne&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;Member Code="IW" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Income&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Revenu&lt;/Name&gt;&lt;ChildMember Code="IW_HADI" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Household net adjusted disposable income&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Revenu disponible ajusté net des ménages&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="IW_HNFW" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Household net wealth&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Patrimoine net des ménages&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;Member Code="JE" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Jobs&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Emploi&lt;/Name&gt;&lt;ChildMember Code="JE_LMIS" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Labour market insecurity&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Insécurité sur le marché du travail&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="JE_EMPL" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Employment rate&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Taux d’emploi&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="JE_LTUR" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Long-term unemployment rate&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Taux de chômage de longue durée&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="JE_PEARN" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Personal earnings&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Revenus moyens d’activité&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;Member Code="SC" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Community&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Liens sociaux&lt;/Name&gt;&lt;ChildMember Code="SC_SNTWS" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Quality of support network&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Qualité du réseau social&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;Member Code="ES" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Education&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Enseignement&lt;/Name&gt;&lt;ChildMember Code="ES_EDUA" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Educational attainment&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Niveau d’instruction&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="ES_STCS" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Student skills&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Compétences des élèves&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="ES_EDUEX" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Years in education&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Années de scolarité&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;Member Code="EQ" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Environment&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Environnement&lt;/Name&gt;&lt;ChildMember Code="EQ_AIRP" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Air pollution&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Pollution atmosphérique&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="EQ_WATER" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Water quality&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Qualité de l’eau&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;Member Code="CG" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Civic engagement&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Engagement civique&lt;/Name&gt;&lt;ChildMember Code="CG_SENG" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Stakeholder engagement for developing regulations&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Participation des parties prenantes à l’élaboration de la réglementation&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="CG_VOTO" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Voter turnout&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Participation électorale&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;Member Code="HS" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Health&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Santé&lt;/Name&gt;&lt;ChildMember Code="HS_LEB" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Life expectancy&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Espérance de vie&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="HS_SFRH" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Self-reported health&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Auto-évaluation de l’état de santé&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;Member Code="SW" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Life Satisfaction&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Satisfaction&lt;/Name&gt;&lt;ChildMember Code="SW_LIFS" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Life satisfaction&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Satisfaction à l’égard de la vie&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;Member Code="PS" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Safety&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Sécurité&lt;/Name&gt;&lt;ChildMember Code="PS_FSAFEN" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Feeling safe walking alone at night&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Se sentir en sécurité quand on marche seul la nuit&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="PS_REPH" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Homicide rate&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Taux d’homicides&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;Member Code="WL" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="1"&gt;&lt;Name LocaleIsoCode="en"&gt;Work-Life Balance&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Équilibre travail-vie&lt;/Name&gt;&lt;ChildMember Code="WL_EWLH" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Employees working very long hours&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Horaires de travail lourds&lt;/Name&gt;&lt;/ChildMember&gt;&lt;ChildMember Code="WL_TNOW" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Time devoted to leisure and personal care&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Temps consacré aux loisirs et à soi&lt;/Name&gt;&lt;/ChildMember&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="MEASURE" HasMetadata="false" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Measure&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Mesure&lt;/Name&gt;&lt;Member Code="L" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Value&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Valeur&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="INEQUALITY" HasMetadata="false" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Inequality&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Inégalité&lt;/Name&gt;&lt;Member Code="TOT" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Total&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Total&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="MN" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Men&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Homme&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="WMN" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Women&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Femme&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="HGH" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;High&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Haut&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="LW" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Low&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Bas&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Tabulation Axis="horizontal"&gt;&lt;Dimension Code="INDICATOR" /&gt;&lt;/Tabulation&gt;&lt;Tabulation Axis="vertical"&gt;&lt;Dimension Code="LOCATION" CommonCode="LOCATION" /&gt;&lt;/Tabulation&gt;&lt;Tabulation Axis="page"&gt;&lt;Dimension Code="INEQUALITY" /&gt;&lt;Dimension Code="MEASURE" /&gt;&lt;/Tabulation&gt;&lt;Formatting&gt;&lt;Labels LocaleIsoCode="en" /&gt;&lt;Power&gt;0&lt;/Power&gt;&lt;Decimals&gt;-1&lt;/Decimals&gt;&lt;SkipEmptyLines&gt;true&lt;/SkipEmptyLines&gt;&lt;SkipEmptyCols&gt;false&lt;/SkipEmptyCols&gt;&lt;SkipLineHierarchy&gt;false&lt;/SkipLineHierarchy&gt;&lt;SkipColHierarchy&gt;false&lt;/SkipColHierarchy&gt;&lt;Page&gt;1&lt;/Page&gt;&lt;/Formatting&gt;&lt;/DataTable&gt;&lt;Format&gt;&lt;ShowEmptyAxes&gt;true&lt;/ShowEmptyAxes&gt;&lt;Page&gt;1&lt;/Page&gt;&lt;EnableSort&gt;true&lt;/EnableSort&gt;&lt;IncludeFlagColumn&gt;false&lt;/IncludeFlagColumn&gt;&lt;IncludeTimeSeriesId&gt;false&lt;/IncludeTimeSeriesId&gt;&lt;DoBarChart&gt;false&lt;/DoBarChart&gt;&lt;FreezePanes&gt;true&lt;/FreezePanes&gt;&lt;MaxBarChartLen&gt;65&lt;/MaxBarChartLen&gt;&lt;/Format&gt;&lt;Query&gt;&lt;AbsoluteUri&gt;http://stats.oecd.org//View.aspx?QueryId=86595&amp;amp;QueryType=Public&amp;amp;Lang=en&lt;/AbsoluteUri&gt;&lt;/Query&gt;&lt;/WebTableParameter&gt;</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t>Turkey</t>
+  </si>
+  <si>
+    <t>South Korea</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -5142,8 +5145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -6673,7 +6676,7 @@
     </row>
     <row r="19" spans="1:27" ht="15">
       <c r="A19" s="19" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>70</v>
@@ -6925,7 +6928,7 @@
         <v>117</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="C22" s="16">
         <v>2.5</v>

</xml_diff>